<commit_message>
Update weights loop. Test run changes
</commit_message>
<xml_diff>
--- a/ActivationFunctions/PLU.xlsx
+++ b/ActivationFunctions/PLU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\NeuralNetwork\ActivationFunctions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2180FC0F-8CD2-4E93-9309-8FB4E7FD22BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD042DB7-1E9C-4134-BEEF-C90258440BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3990" yWindow="3270" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -269,127 +269,127 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>0.95499999999999996</c:v>
+                  <c:v>1.0900000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.95</c:v>
+                  <c:v>1.085</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.94499999999999995</c:v>
+                  <c:v>1.08</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.94</c:v>
+                  <c:v>1.075</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.93499999999999994</c:v>
+                  <c:v>1.07</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.92999999999999994</c:v>
+                  <c:v>1.0649999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.92500000000000004</c:v>
+                  <c:v>1.06</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.91999999999999993</c:v>
+                  <c:v>1.0549999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.91500000000000004</c:v>
+                  <c:v>1.05</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.91</c:v>
+                  <c:v>1.0449999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.90500000000000003</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.9</c:v>
+                  <c:v>1.0349999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.8</c:v>
+                  <c:v>1.03</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.70000000000000007</c:v>
+                  <c:v>1.0249999999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.60000000000000009</c:v>
+                  <c:v>1.02</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>1.0149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.01</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.0049999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.30000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-0.1</c:v>
+                  <c:v>-0.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-0.2</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-0.30000000000000004</c:v>
+                  <c:v>-1.0049999999999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-0.4</c:v>
+                  <c:v>-1.01</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-0.5</c:v>
+                  <c:v>-1.0149999999999999</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-0.60000000000000009</c:v>
+                  <c:v>-1.02</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-0.70000000000000007</c:v>
+                  <c:v>-1.0249999999999999</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-0.8</c:v>
+                  <c:v>-1.03</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-0.9</c:v>
+                  <c:v>-1.0349999999999999</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-0.90500000000000003</c:v>
+                  <c:v>-1.04</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-0.91</c:v>
+                  <c:v>-1.0449999999999999</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-0.91500000000000004</c:v>
+                  <c:v>-1.05</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-0.91999999999999993</c:v>
+                  <c:v>-1.0549999999999999</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-0.92500000000000004</c:v>
+                  <c:v>-1.06</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-0.92999999999999994</c:v>
+                  <c:v>-1.0649999999999999</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-0.93499999999999994</c:v>
+                  <c:v>-1.07</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-0.94</c:v>
+                  <c:v>-1.075</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-0.94499999999999995</c:v>
+                  <c:v>-1.08</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-0.95</c:v>
+                  <c:v>-1.085</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-0.95499999999999996</c:v>
+                  <c:v>-1.0900000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -675,61 +675,61 @@
                   <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>0.01</c:v>
@@ -1328,7 +1328,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1339,7 +1339,7 @@
       </c>
       <c r="B1">
         <f>SIGN(A1)*MIN($E$1*ABS(A1), ($E$2*ABS(A1))+$E$6)</f>
-        <v>0.95499999999999996</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="C1">
         <f xml:space="preserve"> IF(ABS(A1)&gt;$E$5, $E$2, $E$1)</f>
@@ -1349,7 +1349,7 @@
         <v>1</v>
       </c>
       <c r="E1">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1358,7 +1358,7 @@
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B41" si="0">SIGN(A2)*MIN($E$1*ABS(A2), ($E$2*ABS(A2))+$E$6)</f>
-        <v>0.95</v>
+        <v>1.085</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C41" si="1" xml:space="preserve"> IF(ABS(A2)&gt;$E$5, $E$2, $E$1)</f>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="B3">
         <f t="shared" si="0"/>
-        <v>0.94499999999999995</v>
+        <v>1.08</v>
       </c>
       <c r="C3">
         <f t="shared" si="1"/>
@@ -1387,7 +1387,7 @@
         <v>3</v>
       </c>
       <c r="E3">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1396,7 +1396,7 @@
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>0.94</v>
+        <v>1.075</v>
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>0.93499999999999994</v>
+        <v>1.07</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
@@ -1421,7 +1421,7 @@
       </c>
       <c r="E5">
         <f>E3/E1</f>
-        <v>4.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1430,7 +1430,7 @@
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>0.92999999999999994</v>
+        <v>1.0649999999999999</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="E6">
         <f>E3*(1-(E2/E1))</f>
-        <v>0.85499999999999998</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1450,7 +1450,7 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>0.92500000000000004</v>
+        <v>1.06</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>0.91999999999999993</v>
+        <v>1.0549999999999999</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
@@ -1476,7 +1476,7 @@
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>0.91500000000000004</v>
+        <v>1.05</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
@@ -1489,7 +1489,7 @@
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>0.91</v>
+        <v>1.0449999999999999</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
@@ -1502,7 +1502,7 @@
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>0.90500000000000003</v>
+        <v>1.04</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
@@ -1515,11 +1515,11 @@
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>0.9</v>
+        <v>1.0349999999999999</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1528,11 +1528,11 @@
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>1.03</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1541,11 +1541,11 @@
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>0.70000000000000007</v>
+        <v>1.0249999999999999</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1554,11 +1554,11 @@
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>0.60000000000000009</v>
+        <v>1.02</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1567,11 +1567,11 @@
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1.0149999999999999</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1580,11 +1580,11 @@
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>1.01</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1593,11 +1593,11 @@
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
+        <v>1.0049999999999999</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1606,11 +1606,11 @@
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1619,11 +1619,11 @@
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="C20">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1636,7 +1636,7 @@
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1645,11 +1645,11 @@
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>-0.1</v>
+        <v>-0.5</v>
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1658,11 +1658,11 @@
       </c>
       <c r="B23">
         <f>SIGN(A23)*MIN($E$1*ABS(A23), ($E$2*ABS(A23))+$E$6)</f>
-        <v>-0.2</v>
+        <v>-1</v>
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1671,11 +1671,11 @@
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>-0.30000000000000004</v>
+        <v>-1.0049999999999999</v>
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1684,11 +1684,11 @@
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>-0.4</v>
+        <v>-1.01</v>
       </c>
       <c r="C25">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1697,11 +1697,11 @@
       </c>
       <c r="B26">
         <f t="shared" si="0"/>
-        <v>-0.5</v>
+        <v>-1.0149999999999999</v>
       </c>
       <c r="C26">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1710,11 +1710,11 @@
       </c>
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>-0.60000000000000009</v>
+        <v>-1.02</v>
       </c>
       <c r="C27">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1723,11 +1723,11 @@
       </c>
       <c r="B28">
         <f>SIGN(A28)*MIN($E$1*ABS(A28), ($E$2*ABS(A28))+$E$6)</f>
-        <v>-0.70000000000000007</v>
+        <v>-1.0249999999999999</v>
       </c>
       <c r="C28">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1736,11 +1736,11 @@
       </c>
       <c r="B29">
         <f t="shared" si="0"/>
-        <v>-0.8</v>
+        <v>-1.03</v>
       </c>
       <c r="C29">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1749,11 +1749,11 @@
       </c>
       <c r="B30">
         <f t="shared" si="0"/>
-        <v>-0.9</v>
+        <v>-1.0349999999999999</v>
       </c>
       <c r="C30">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1762,7 +1762,7 @@
       </c>
       <c r="B31">
         <f t="shared" si="0"/>
-        <v>-0.90500000000000003</v>
+        <v>-1.04</v>
       </c>
       <c r="C31">
         <f t="shared" si="1"/>
@@ -1775,7 +1775,7 @@
       </c>
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>-0.91</v>
+        <v>-1.0449999999999999</v>
       </c>
       <c r="C32">
         <f t="shared" si="1"/>
@@ -1788,7 +1788,7 @@
       </c>
       <c r="B33">
         <f t="shared" si="0"/>
-        <v>-0.91500000000000004</v>
+        <v>-1.05</v>
       </c>
       <c r="C33">
         <f t="shared" si="1"/>
@@ -1801,7 +1801,7 @@
       </c>
       <c r="B34">
         <f t="shared" si="0"/>
-        <v>-0.91999999999999993</v>
+        <v>-1.0549999999999999</v>
       </c>
       <c r="C34">
         <f t="shared" si="1"/>
@@ -1814,7 +1814,7 @@
       </c>
       <c r="B35">
         <f t="shared" si="0"/>
-        <v>-0.92500000000000004</v>
+        <v>-1.06</v>
       </c>
       <c r="C35">
         <f t="shared" si="1"/>
@@ -1827,7 +1827,7 @@
       </c>
       <c r="B36">
         <f t="shared" si="0"/>
-        <v>-0.92999999999999994</v>
+        <v>-1.0649999999999999</v>
       </c>
       <c r="C36">
         <f t="shared" si="1"/>
@@ -1840,7 +1840,7 @@
       </c>
       <c r="B37">
         <f t="shared" si="0"/>
-        <v>-0.93499999999999994</v>
+        <v>-1.07</v>
       </c>
       <c r="C37">
         <f t="shared" si="1"/>
@@ -1853,7 +1853,7 @@
       </c>
       <c r="B38">
         <f t="shared" si="0"/>
-        <v>-0.94</v>
+        <v>-1.075</v>
       </c>
       <c r="C38">
         <f t="shared" si="1"/>
@@ -1866,7 +1866,7 @@
       </c>
       <c r="B39">
         <f t="shared" si="0"/>
-        <v>-0.94499999999999995</v>
+        <v>-1.08</v>
       </c>
       <c r="C39">
         <f t="shared" si="1"/>
@@ -1879,7 +1879,7 @@
       </c>
       <c r="B40">
         <f t="shared" si="0"/>
-        <v>-0.95</v>
+        <v>-1.085</v>
       </c>
       <c r="C40">
         <f t="shared" si="1"/>
@@ -1892,7 +1892,7 @@
       </c>
       <c r="B41">
         <f t="shared" si="0"/>
-        <v>-0.95499999999999996</v>
+        <v>-1.0900000000000001</v>
       </c>
       <c r="C41">
         <f t="shared" si="1"/>

</xml_diff>